<commit_message>
Test: removed spurious character from CRYPTO22280.xlsx
</commit_message>
<xml_diff>
--- a/test/HMRC-Examples/CRYPTO22280.xlsx
+++ b/test/HMRC-Examples/CRYPTO22280.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottgreen/Development/BittyTaxRelease/BittyTax/test/HMRC-Examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8C08E9-41A4-4A41-80BB-774685435086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E01853-04EA-AC40-AE07-3A09F1824977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9580" yWindow="4540" windowWidth="38980" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Trade</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>Terri decides to sell 1,000 of the tokens for £5,000. The transaction requires that she pays a fee of 0.1% of what she is selling, i.e. 1 token.</t>
-  </si>
-  <si>
-    <t>§</t>
   </si>
 </sst>
 </file>
@@ -156,15 +153,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -173,18 +169,12 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF000000"/>
       </font>
       <numFmt numFmtId="164" formatCode="#,##0.##############################"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -562,11 +552,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -576,7 +566,7 @@
     <col min="3" max="4" width="9.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
     <col min="6" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="9" customWidth="1"/>
     <col min="9" max="10" width="9.6640625" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
     <col min="12" max="12" width="19.6640625" customWidth="1"/>
@@ -613,7 +603,7 @@
       <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -632,7 +622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -645,7 +635,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -736,34 +726,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H17" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="B4:B5">
-    <cfRule type="expression" dxfId="9" priority="34">
+    <cfRule type="expression" dxfId="7" priority="34">
       <formula>INT(B4)=B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="expression" dxfId="8" priority="35">
+    <cfRule type="expression" dxfId="6" priority="35">
       <formula>INT(E4)=E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="6" priority="31">
+    <cfRule type="expression" dxfId="5" priority="31">
       <formula>INT(E5)=E5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="5" priority="22">
+    <cfRule type="expression" dxfId="4" priority="22">
       <formula>INT(B3)=B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="4" priority="23">
+    <cfRule type="expression" dxfId="3" priority="23">
       <formula>INT(E3)=E3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>